<commit_message>
should all be fixed
</commit_message>
<xml_diff>
--- a/metadata/2022/hwb_metadata_p7_row_names.xlsx
+++ b/metadata/2022/hwb_metadata_p7_row_names.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://scotsconnect-my.sharepoint.com/personal/victoria_dunn_gov_scot/Documents/Git Repos/HWB Rap Project/hwb-census/metadata/2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="67" documentId="13_ncr:1_{42891873-95E1-4EC8-B22F-432915EC2EDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00F1AC09-9945-460D-A72B-5B6DB23C70EA}"/>
+  <xr:revisionPtr revIDLastSave="69" documentId="13_ncr:1_{42891873-95E1-4EC8-B22F-432915EC2EDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3E498BB8-029A-42D4-8FCD-305A7FA6F7E2}"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{E38ABFA0-70CD-4F29-8370-4B8A66B5B812}"/>
+    <workbookView xWindow="14940" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{E38ABFA0-70CD-4F29-8370-4B8A66B5B812}"/>
   </bookViews>
   <sheets>
     <sheet name="P7" sheetId="1" r:id="rId1"/>
@@ -221,9 +221,6 @@
     <t>None at all</t>
   </si>
   <si>
-    <t>Some time (up to 2 hours a day)</t>
-  </si>
-  <si>
     <t>Quite a bit of time (about 3 hours a day or more)</t>
   </si>
   <si>
@@ -696,6 +693,9 @@
   </si>
   <si>
     <t>play_areas_outdoors</t>
+  </si>
+  <si>
+    <t>Some time (up to about 2 hours a day)</t>
   </si>
 </sst>
 </file>
@@ -731,11 +731,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1056,344 +1053,344 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:DE17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CF1" workbookViewId="0">
-      <selection activeCell="DE1" sqref="DE1"/>
+    <sheetView tabSelected="1" topLeftCell="AL1" workbookViewId="0">
+      <selection activeCell="BA3" sqref="BA3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:109" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B1" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="BA1" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BB1" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BC1" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="BC1" s="1" t="s">
+      <c r="BD1" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BE1" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BF1" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="BF1" s="1" t="s">
+      <c r="BG1" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="BG1" s="1" t="s">
+      <c r="BH1" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="BH1" s="1" t="s">
+      <c r="BI1" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="BI1" s="1" t="s">
+      <c r="BJ1" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="BJ1" s="1" t="s">
+      <c r="BK1" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="BK1" s="1" t="s">
+      <c r="BL1" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="BL1" s="1" t="s">
+      <c r="BM1" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="BM1" s="1" t="s">
+      <c r="BN1" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="BN1" s="1" t="s">
+      <c r="BO1" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="BO1" s="1" t="s">
+      <c r="BP1" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="BP1" s="1" t="s">
+      <c r="BQ1" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="BQ1" s="1" t="s">
+      <c r="BR1" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="BR1" s="1" t="s">
+      <c r="BS1" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="BS1" s="1" t="s">
+      <c r="BT1" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="BT1" s="1" t="s">
+      <c r="BU1" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="BU1" s="1" t="s">
+      <c r="BV1" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="BV1" s="1" t="s">
+      <c r="BW1" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="BW1" s="1" t="s">
+      <c r="BX1" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="BX1" s="1" t="s">
+      <c r="BY1" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="BY1" s="1" t="s">
+      <c r="BZ1" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="BZ1" s="1" t="s">
+      <c r="CA1" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="CA1" s="1" t="s">
+      <c r="CB1" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="CB1" s="1" t="s">
+      <c r="CC1" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="CC1" s="1" t="s">
+      <c r="CD1" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="CD1" s="1" t="s">
+      <c r="CE1" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="CE1" s="1" t="s">
+      <c r="CF1" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="CF1" s="1" t="s">
+      <c r="CG1" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="CG1" s="1" t="s">
+      <c r="CH1" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="CH1" s="1" t="s">
+      <c r="CI1" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="CI1" s="1" t="s">
+      <c r="CJ1" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="CJ1" s="1" t="s">
+      <c r="CK1" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="CK1" s="1" t="s">
+      <c r="CL1" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="CL1" s="1" t="s">
+      <c r="CM1" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="CM1" s="1" t="s">
+      <c r="CN1" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="CN1" s="1" t="s">
+      <c r="CO1" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="CO1" s="1" t="s">
+      <c r="CP1" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="CP1" s="1" t="s">
+      <c r="CQ1" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="CQ1" s="1" t="s">
+      <c r="CR1" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="CR1" s="1" t="s">
+      <c r="CS1" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="CS1" s="1" t="s">
+      <c r="CT1" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="CT1" s="1" t="s">
+      <c r="CU1" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="CU1" s="1" t="s">
+      <c r="CV1" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="CV1" s="1" t="s">
+      <c r="CW1" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="CW1" s="1" t="s">
+      <c r="CX1" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="CX1" s="1" t="s">
+      <c r="CY1" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="CY1" s="1" t="s">
+      <c r="CZ1" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="CZ1" s="1" t="s">
+      <c r="DA1" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="DA1" s="1" t="s">
+      <c r="DB1" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="DB1" s="1" t="s">
+      <c r="DC1" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="DC1" s="1" t="s">
+      <c r="DD1" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="DD1" s="1" t="s">
+      <c r="DE1" s="1" t="s">
         <v>218</v>
-      </c>
-      <c r="DE1" s="1" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="2" spans="1:109" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B2" t="s">
         <v>30</v>
@@ -1600,10 +1597,10 @@
         <v>0</v>
       </c>
       <c r="BT2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="BU2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="BV2" t="s">
         <v>30</v>
@@ -1639,13 +1636,13 @@
         <v>30</v>
       </c>
       <c r="CG2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="CH2" t="s">
         <v>30</v>
       </c>
       <c r="CI2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="CJ2" t="s">
         <v>7</v>
@@ -1663,60 +1660,60 @@
         <v>19</v>
       </c>
       <c r="CO2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="CP2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="CQ2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="CR2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="CS2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="CT2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="CU2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="CV2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="CW2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="CX2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="CY2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="CZ2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="DA2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="DB2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="DC2" t="s">
         <v>57</v>
       </c>
       <c r="DD2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="DE2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:109" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B3" t="s">
         <v>31</v>
@@ -1863,10 +1860,10 @@
         <v>31</v>
       </c>
       <c r="AZ3" t="s">
-        <v>61</v>
+        <v>219</v>
       </c>
       <c r="BA3" t="s">
-        <v>61</v>
+        <v>219</v>
       </c>
       <c r="BB3" t="s">
         <v>31</v>
@@ -1893,7 +1890,7 @@
         <v>31</v>
       </c>
       <c r="BJ3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="BK3" t="s">
         <v>1</v>
@@ -1962,19 +1959,19 @@
         <v>31</v>
       </c>
       <c r="CG3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="CH3" t="s">
         <v>31</v>
       </c>
       <c r="CI3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="CJ3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="CK3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="CL3" t="s">
         <v>35</v>
@@ -1983,63 +1980,63 @@
         <v>31</v>
       </c>
       <c r="CN3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="CO3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="CP3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="CQ3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="CR3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="CS3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="CT3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="CU3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="CV3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="CW3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="CX3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="CY3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="CZ3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="DA3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="DB3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="DC3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="DD3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="DE3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:109" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -2186,10 +2183,10 @@
         <v>5</v>
       </c>
       <c r="AZ4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="BA4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="BB4" t="s">
         <v>6</v>
@@ -2216,7 +2213,7 @@
         <v>6</v>
       </c>
       <c r="BJ4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="BK4" t="s">
         <v>2</v>
@@ -2246,7 +2243,7 @@
         <v>2</v>
       </c>
       <c r="BT4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="BU4" t="s">
         <v>35</v>
@@ -2285,19 +2282,19 @@
         <v>6</v>
       </c>
       <c r="CG4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="CH4" t="s">
         <v>5</v>
       </c>
       <c r="CI4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="CJ4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="CK4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="CL4" t="s">
         <v>58</v>
@@ -2306,55 +2303,55 @@
         <v>5</v>
       </c>
       <c r="CN4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="CO4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="CP4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="CQ4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="CR4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="CS4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="CT4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="CU4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="CV4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="CW4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="CX4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="CY4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="CZ4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="DA4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="DB4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="DC4" t="s">
         <v>58</v>
       </c>
       <c r="DD4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="DE4" t="s">
         <v>31</v>
@@ -2362,10 +2359,10 @@
     </row>
     <row r="5" spans="1:109" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E5" t="s">
         <v>3</v>
@@ -2515,31 +2512,31 @@
         <v>6</v>
       </c>
       <c r="BB5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="BC5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="BD5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="BE5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="BF5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="BG5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="BH5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="BI5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="BJ5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="BK5" t="s">
         <v>3</v>
@@ -2578,37 +2575,37 @@
         <v>6</v>
       </c>
       <c r="BW5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="BX5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="BY5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="BZ5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="CA5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="CB5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="CC5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="CD5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="CE5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="CF5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="CG5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="CH5" t="s">
         <v>6</v>
@@ -2617,10 +2614,10 @@
         <v>5</v>
       </c>
       <c r="CJ5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="CK5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="CL5" t="s">
         <v>25</v>
@@ -2674,7 +2671,7 @@
         <v>6</v>
       </c>
       <c r="DC5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="DD5" t="s">
         <v>5</v>
@@ -2685,7 +2682,7 @@
     </row>
     <row r="6" spans="1:109" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E6" t="s">
         <v>4</v>
@@ -2733,7 +2730,7 @@
         <v>5</v>
       </c>
       <c r="T6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="U6" t="s">
         <v>4</v>
@@ -2826,13 +2823,13 @@
         <v>6</v>
       </c>
       <c r="AY6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AZ6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="BA6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="BJ6" t="s">
         <v>5</v>
@@ -2871,19 +2868,19 @@
         <v>6</v>
       </c>
       <c r="BV6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="CG6" t="s">
         <v>25</v>
       </c>
       <c r="CH6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="CI6" t="s">
         <v>6</v>
       </c>
       <c r="CJ6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="CK6" t="s">
         <v>25</v>
@@ -2892,7 +2889,7 @@
         <v>5</v>
       </c>
       <c r="CM6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="CN6" t="s">
         <v>6</v>
@@ -2901,43 +2898,43 @@
         <v>6</v>
       </c>
       <c r="CP6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="CQ6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="CR6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="CS6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="CT6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="CU6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="CV6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="CW6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="CX6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="CY6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="CZ6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="DA6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="DB6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="DC6" t="s">
         <v>5</v>
@@ -2951,7 +2948,7 @@
     </row>
     <row r="7" spans="1:109" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E7" t="s">
         <v>5</v>
@@ -2987,7 +2984,7 @@
         <v>6</v>
       </c>
       <c r="P7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Q7" t="s">
         <v>5</v>
@@ -3047,7 +3044,7 @@
         <v>6</v>
       </c>
       <c r="AK7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AL7" t="s">
         <v>6</v>
@@ -3083,10 +3080,10 @@
         <v>6</v>
       </c>
       <c r="AW7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AX7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="BJ7" t="s">
         <v>6</v>
@@ -3119,16 +3116,16 @@
         <v>6</v>
       </c>
       <c r="BT7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="BU7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="CG7" t="s">
         <v>5</v>
       </c>
       <c r="CI7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="CJ7" t="s">
         <v>5</v>
@@ -3140,24 +3137,24 @@
         <v>6</v>
       </c>
       <c r="CN7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="CO7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="DC7" t="s">
         <v>6</v>
       </c>
       <c r="DD7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="DE7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:109" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E8" t="s">
         <v>6</v>
@@ -3190,7 +3187,7 @@
         <v>6</v>
       </c>
       <c r="O8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Q8" t="s">
         <v>6</v>
@@ -3199,7 +3196,7 @@
         <v>25</v>
       </c>
       <c r="S8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="U8" t="s">
         <v>6</v>
@@ -3211,28 +3208,28 @@
         <v>6</v>
       </c>
       <c r="X8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Y8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Z8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AA8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AB8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AC8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AD8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AE8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AF8" t="s">
         <v>6</v>
@@ -3247,70 +3244,70 @@
         <v>6</v>
       </c>
       <c r="AJ8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AL8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AM8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AN8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AO8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AP8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AQ8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AR8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AS8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AT8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AU8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AV8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="BJ8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="BK8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="BL8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="BM8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="BN8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="BO8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="BP8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="BQ8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="BR8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="BS8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="CG8" t="s">
         <v>6</v>
@@ -3322,86 +3319,86 @@
         <v>6</v>
       </c>
       <c r="CL8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="DC8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:109" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="N9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Q9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="R9" t="s">
         <v>5</v>
       </c>
       <c r="U9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="V9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="W9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AF9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AG9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AH9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AI9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="CG9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="CJ9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="CK9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:109" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="R10" t="s">
         <v>6</v>
@@ -3409,40 +3406,40 @@
     </row>
     <row r="11" spans="1:109" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="R11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:109" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:109" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" spans="1:109" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="15" spans="1:109" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="16" spans="1:109" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>